<commit_message>
level fail & level complete (attempts currently not working)
</commit_message>
<xml_diff>
--- a/Vocabulary/GBLxAPI_Vocab_User.xlsx
+++ b/Vocabulary/GBLxAPI_Vocab_User.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siritembunkiart/Documents/Side Projects/MMI/Martian-Music-Invasion/Vocabulary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F5D7AF-3B4B-FD42-A0CC-AA1F233320D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59CE507-0723-8B41-B732-21D65C4929B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
   <si>
     <t>URI</t>
   </si>
@@ -43,7 +43,19 @@
     <t>cutsceneAudioFinished</t>
   </si>
   <si>
-    <t>http://www.martianmusicinvasion.com/extensions/cutsceneAudioFinished</t>
+    <t>levelAttempts</t>
+  </si>
+  <si>
+    <t>http://www.martianmusicinvasion.com/game/extensions/cutsceneAudioFinished</t>
+  </si>
+  <si>
+    <t>http://www.martianmusicinvasion.com/game/extensions/levelAttempts</t>
+  </si>
+  <si>
+    <t>livesLeft</t>
+  </si>
+  <si>
+    <t>http://www.martianmusicinvasion.com/game/extensions/cutsceneAudioFinished/livesLeft</t>
   </si>
 </sst>
 </file>
@@ -1284,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C44E092-9311-D343-AD6A-E3CAD463F99E}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1313,12 +1325,30 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{3EBED3E0-B660-FD4A-8094-03EAD7A2E13E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{BF3AB070-1455-E04D-8562-CB849D57A6E3}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{86AE8064-1828-A049-95B0-5FED82FD2E22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2859,12 +2889,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3039,15 +3066,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3072,10 +3103,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>